<commit_message>
CHG: updated order list
</commit_message>
<xml_diff>
--- a/eagle/Bestellliste.xlsx
+++ b/eagle/Bestellliste.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\eagle\Radio V2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\fhradiov2\eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="144">
   <si>
     <t>FH-Radio Bestellliste</t>
   </si>
@@ -181,18 +181,12 @@
     <t>IRF7309</t>
   </si>
   <si>
-    <t>LP38693</t>
-  </si>
-  <si>
     <t>MPS430G2553</t>
   </si>
   <si>
     <t>PCA8574</t>
   </si>
   <si>
-    <t>PCA9530</t>
-  </si>
-  <si>
     <t>PEC11R</t>
   </si>
   <si>
@@ -364,15 +358,9 @@
     <t>771-PCA85PW118</t>
   </si>
   <si>
-    <t>771-PCA9530D118</t>
-  </si>
-  <si>
     <t>SO8</t>
   </si>
   <si>
-    <t>652-PEC11R-4130F-S18</t>
-  </si>
-  <si>
     <t>59 F 2100</t>
   </si>
   <si>
@@ -388,9 +376,6 @@
     <t>595-P430G2553IRHB32R</t>
   </si>
   <si>
-    <t>926-38693SD-ADJ/NOPB</t>
-  </si>
-  <si>
     <t>Order Number Reichelt</t>
   </si>
   <si>
@@ -476,13 +461,34 @@
   </si>
   <si>
     <t>74 D 3158</t>
+  </si>
+  <si>
+    <t>PCA9632</t>
+  </si>
+  <si>
+    <t>771-PCA9632DP1118</t>
+  </si>
+  <si>
+    <t>926-LP38693SD33NOPB</t>
+  </si>
+  <si>
+    <t>LP38693-3.3</t>
+  </si>
+  <si>
+    <t>652-PEC11R-4225F-S24</t>
+  </si>
+  <si>
+    <t>595-OPT3001DNPT</t>
+  </si>
+  <si>
+    <t>OPT3001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +503,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -520,7 +532,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -531,6 +543,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -812,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,13 +859,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
@@ -865,19 +879,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -890,16 +904,16 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -911,7 +925,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -919,7 +933,7 @@
         <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -934,10 +948,10 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -953,13 +967,13 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G8" t="s">
         <v>22</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -971,15 +985,15 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -991,20 +1005,20 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="1"/>
       <c r="G10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
@@ -1013,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="1"/>
@@ -1021,7 +1035,7 @@
         <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1035,7 +1049,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="1"/>
@@ -1043,7 +1057,7 @@
         <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1057,7 +1071,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="1"/>
@@ -1065,7 +1079,7 @@
         <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1079,7 +1093,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="1"/>
@@ -1087,7 +1101,7 @@
         <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1101,7 +1115,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="1"/>
@@ -1109,7 +1123,7 @@
         <v>18</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1123,7 +1137,7 @@
         <v>20</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
@@ -1131,7 +1145,7 @@
         <v>9</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1145,7 +1159,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
@@ -1153,7 +1167,7 @@
         <v>9</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1161,19 +1175,19 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="3" t="s">
-        <v>112</v>
+      <c r="F18" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1181,19 +1195,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1201,19 +1215,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1221,19 +1235,19 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="3" t="s">
-        <v>104</v>
+      <c r="F21" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="G21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1241,19 +1255,19 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="3" t="s">
-        <v>106</v>
+      <c r="F22" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="G22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1265,7 +1279,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
@@ -1273,7 +1287,7 @@
         <v>6</v>
       </c>
       <c r="H23" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1285,15 +1299,15 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H24" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1309,13 +1323,13 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G25" t="s">
         <v>24</v>
       </c>
       <c r="H25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1333,7 +1347,7 @@
         <v>7</v>
       </c>
       <c r="H26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1347,7 +1361,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>
@@ -1355,7 +1369,7 @@
         <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1366,10 +1380,10 @@
         <v>33</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1377,7 +1391,7 @@
         <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1388,10 +1402,10 @@
         <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1399,7 +1413,7 @@
         <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1410,10 +1424,10 @@
         <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1421,7 +1435,7 @@
         <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1429,19 +1443,19 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1455,13 +1469,13 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G32" t="s">
         <v>8</v>
       </c>
       <c r="H32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1473,7 +1487,7 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="1"/>
@@ -1481,7 +1495,7 @@
         <v>21</v>
       </c>
       <c r="H33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1489,19 +1503,19 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1515,7 +1529,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="1"/>
@@ -1523,12 +1537,12 @@
         <v>11</v>
       </c>
       <c r="H35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
@@ -1537,7 +1551,7 @@
         <v>15</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="1"/>
@@ -1545,7 +1559,7 @@
         <v>11</v>
       </c>
       <c r="H36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1559,7 +1573,7 @@
         <v>200</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="1"/>
@@ -1567,7 +1581,7 @@
         <v>11</v>
       </c>
       <c r="H37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1581,7 +1595,7 @@
         <v>4.7</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="1"/>
@@ -1589,7 +1603,7 @@
         <v>11</v>
       </c>
       <c r="H38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1603,7 +1617,7 @@
         <v>25</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="1"/>
@@ -1611,7 +1625,7 @@
         <v>11</v>
       </c>
       <c r="H39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1631,7 +1645,7 @@
         <v>11</v>
       </c>
       <c r="H40" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1639,19 +1653,30 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H41" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>SUM(A4:A41)</f>
-        <v>107</v>
+        <v>1</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f>SUM(A4:A42)</f>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1676,23 +1701,24 @@
     <hyperlink ref="D9" r:id="rId15" display="https://www.buerklin.com/default.asp?event=ShowArtikel(24S3251)&amp;context=ArtikelSubsetId:0;SE:irf7103;PHNode:SE,vt,0;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_24S3251"/>
     <hyperlink ref="D10" r:id="rId16" display="https://www.buerklin.com/default.asp?event=ShowArtikel(24S3266)&amp;context=ArtikelSubsetId:0;SE:irf7309;PHNode:SE,vt,0;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_24S3266"/>
     <hyperlink ref="F20" r:id="rId17" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/NXP-Semiconductors/PCA8574PW118/?qs=sGAEpiMZZMuFG5L82Zqpsk%252bwjZZ2KBJ9hRx7nZCeYh0%3d"/>
-    <hyperlink ref="F21" r:id="rId18" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/NXP-Semiconductors/PCA9530D118/?qs=sGAEpiMZZMsE420DPIasPmrizm59k0PNUJJgvnyneTI%3d"/>
-    <hyperlink ref="F22" r:id="rId19"/>
-    <hyperlink ref="D23" r:id="rId20" display="https://www.buerklin.com/default.asp?event=ShowArtikel(59F2100)&amp;context=ArtikelSubsetId:0;PHNode:PH,PH,24330;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_59F2100"/>
-    <hyperlink ref="F31" r:id="rId21" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/Texas-Instruments/TPA2016D2RTJR/?qs=sGAEpiMZZMv%2f6jcQNCTArSgvBT18HtHI"/>
-    <hyperlink ref="F32" r:id="rId22" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/Texas-Instruments/TS3A44159RGTR/?qs=sGAEpiMZZMtxrAS98ir%252bs8Sii1%252bdHDwCdOyRrdJ%252bfTw%3d"/>
-    <hyperlink ref="D33" r:id="rId23" display="https://www.buerklin.com/default.asp?event=ShowArtikel(09H3082)&amp;context=ArtikelSubsetId:0;SE:wago%202060;PHNode:SE,hsvt,0;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_09H3082"/>
-    <hyperlink ref="F19" r:id="rId24" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/Texas-Instruments/MSP430G2553IRHB32R/?qs=sGAEpiMZZMsuBfEaN9EhVfuKxkcA8SoY"/>
-    <hyperlink ref="F18" r:id="rId25" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/Texas-Instruments/LP38693SD-ADJ-NOPB/?qs=sGAEpiMZZMvu8NZDyZ4K0WeI8k4vVQJ6"/>
-    <hyperlink ref="E34" r:id="rId26" tooltip="Wannenstecker, 10-polig, gewinkelt" display="http://www.reichelt.de/Pfosten-Wannenstecker/WSL-10W/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=22818&amp;GROUPID=3231&amp;artnr=WSL+10W"/>
-    <hyperlink ref="D6" r:id="rId27" display="https://www.buerklin.com/default.asp?event=ShowArtikel(17S8697)&amp;context=ArtikelSubsetId:0;SE:bss123;PHNode:SE,vt,0;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_17S8697"/>
-    <hyperlink ref="E5" r:id="rId28" tooltip="Schottky Diode SMD, SOT-23, 30V, 0,25A" display="http://www.reichelt.de/BAT-54S-SMD/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=41905&amp;artnr=BAT+54S+SMD&amp;SEARCH=bat54s"/>
-    <hyperlink ref="F5" r:id="rId29" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/Vishay-Semiconductors/BAT54S-E3-08/?qs=sGAEpiMZZMvNv09GOMabneRdrmDZYYtc"/>
-    <hyperlink ref="D4" r:id="rId30" display="https://www.buerklin.com/default.asp?event=ShowArtikel(26S8142)&amp;context=ArtikelSubsetId:0;SE:1N4148;PHNode:SE,vt,0;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_26S8142"/>
-    <hyperlink ref="D24" r:id="rId31" display="https://www.buerklin.com/default.asp?event=ShowArtikel(59F2100)&amp;context=ArtikelSubsetId:0;PHNode:PH,PH,24330;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_59F2100"/>
-    <hyperlink ref="D41" r:id="rId32" display="https://www.buerklin.com/default.asp?event=ShowArtikel(40F4232)&amp;context=ArtikelSubsetId:0;SE:jumper;PHNode:SE,swvt,0;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_40F4232"/>
+    <hyperlink ref="D23" r:id="rId18" display="https://www.buerklin.com/default.asp?event=ShowArtikel(59F2100)&amp;context=ArtikelSubsetId:0;PHNode:PH,PH,24330;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_59F2100"/>
+    <hyperlink ref="F31" r:id="rId19" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/Texas-Instruments/TPA2016D2RTJR/?qs=sGAEpiMZZMv%2f6jcQNCTArSgvBT18HtHI"/>
+    <hyperlink ref="F32" r:id="rId20" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/Texas-Instruments/TS3A44159RGTR/?qs=sGAEpiMZZMtxrAS98ir%252bs8Sii1%252bdHDwCdOyRrdJ%252bfTw%3d"/>
+    <hyperlink ref="D33" r:id="rId21" display="https://www.buerklin.com/default.asp?event=ShowArtikel(09H3082)&amp;context=ArtikelSubsetId:0;SE:wago%202060;PHNode:SE,hsvt,0;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_09H3082"/>
+    <hyperlink ref="F19" r:id="rId22" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/Texas-Instruments/MSP430G2553IRHB32R/?qs=sGAEpiMZZMsuBfEaN9EhVfuKxkcA8SoY"/>
+    <hyperlink ref="E34" r:id="rId23" tooltip="Wannenstecker, 10-polig, gewinkelt" display="http://www.reichelt.de/Pfosten-Wannenstecker/WSL-10W/3/index.html?&amp;ACTION=3&amp;LA=2&amp;ARTICLE=22818&amp;GROUPID=3231&amp;artnr=WSL+10W"/>
+    <hyperlink ref="D6" r:id="rId24" display="https://www.buerklin.com/default.asp?event=ShowArtikel(17S8697)&amp;context=ArtikelSubsetId:0;SE:bss123;PHNode:SE,vt,0;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_17S8697"/>
+    <hyperlink ref="E5" r:id="rId25" tooltip="Schottky Diode SMD, SOT-23, 30V, 0,25A" display="http://www.reichelt.de/BAT-54S-SMD/3/index.html?&amp;ACTION=3&amp;LA=446&amp;ARTICLE=41905&amp;artnr=BAT+54S+SMD&amp;SEARCH=bat54s"/>
+    <hyperlink ref="F5" r:id="rId26" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/Vishay-Semiconductors/BAT54S-E3-08/?qs=sGAEpiMZZMvNv09GOMabneRdrmDZYYtc"/>
+    <hyperlink ref="D4" r:id="rId27" display="https://www.buerklin.com/default.asp?event=ShowArtikel(26S8142)&amp;context=ArtikelSubsetId:0;SE:1N4148;PHNode:SE,vt,0;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_26S8142"/>
+    <hyperlink ref="D24" r:id="rId28" display="https://www.buerklin.com/default.asp?event=ShowArtikel(59F2100)&amp;context=ArtikelSubsetId:0;PHNode:PH,PH,24330;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_59F2100"/>
+    <hyperlink ref="D41" r:id="rId29" display="https://www.buerklin.com/default.asp?event=ShowArtikel(40F4232)&amp;context=ArtikelSubsetId:0;SE:jumper;PHNode:SE,swvt,0;ALArtikelProSeite:100&amp;l=d&amp;jump=ArtNr_40F4232"/>
+    <hyperlink ref="F21" r:id="rId30"/>
+    <hyperlink ref="F18" r:id="rId31" tooltip="Hier klicken, um zusätzliche Informationen über dieses Produkt anzuzeigen." display="http://www.mouser.de/ProductDetail/Texas-Instruments/LP38693SD-33-NOPB/?qs=sGAEpiMZZMsGz1a6aV8DcBojudwDyMGaGjSjQlSYGIY%3d"/>
+    <hyperlink ref="F22" r:id="rId32"/>
+    <hyperlink ref="F42" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>